<commit_message>
Ajuste final nas telas e execução deos testes
</commit_message>
<xml_diff>
--- a/21GRLADS01BDJ10221E31 - AT WEB_ roteiro.xlsx
+++ b/21GRLADS01BDJ10221E31 - AT WEB_ roteiro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6aeb75a1ec44b17d/Área de Trabalho/Bloco Java/003 - Dev Web Java EE/Kakebo_Assessment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{16E0DA88-D65B-470A-A08C-27DEC7EF31B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C19F81B2-C936-447C-8768-FE97D6C48977}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="8_{16E0DA88-D65B-470A-A08C-27DEC7EF31B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3FD4C2E-A4E7-4968-BEE5-D2595D7B8009}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="java web" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -265,7 +265,7 @@
     <t>ENTREGA SEM APRESENTA: QUARTA - 15/12</t>
   </si>
   <si>
-    <t>ok</t>
+    <t>Ok</t>
   </si>
 </sst>
 </file>
@@ -505,6 +505,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -528,24 +546,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -767,8 +767,8 @@
   </sheetPr>
   <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -779,10 +779,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="13" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="34"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -814,7 +814,7 @@
       <c r="U1" s="3"/>
     </row>
     <row r="2" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="27" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4">
@@ -845,7 +845,7 @@
       <c r="U2" s="3"/>
     </row>
     <row r="3" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="6">
         <f t="shared" ref="B3:B51" si="0">B2+1</f>
         <v>2</v>
@@ -875,7 +875,7 @@
       <c r="U3" s="3"/>
     </row>
     <row r="4" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -905,7 +905,7 @@
       <c r="U4" s="3"/>
     </row>
     <row r="5" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="35" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="6">
@@ -937,7 +937,7 @@
       <c r="U5" s="3"/>
     </row>
     <row r="6" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -967,7 +967,7 @@
       <c r="U6" s="3"/>
     </row>
     <row r="7" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -997,7 +997,7 @@
       <c r="U7" s="3"/>
     </row>
     <row r="8" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1027,7 +1027,7 @@
       <c r="U8" s="3"/>
     </row>
     <row r="9" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1057,7 +1057,7 @@
       <c r="U9" s="3"/>
     </row>
     <row r="10" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1087,7 +1087,7 @@
       <c r="U10" s="3"/>
     </row>
     <row r="11" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1117,20 +1117,20 @@
       <c r="U11" s="3"/>
     </row>
     <row r="12" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="31">
+      <c r="A12" s="28"/>
+      <c r="B12" s="21">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1147,7 +1147,7 @@
       <c r="U12" s="3"/>
     </row>
     <row r="13" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="27" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="6">
@@ -1157,7 +1157,7 @@
       <c r="C13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="26" t="s">
         <v>77</v>
       </c>
       <c r="E13" s="8"/>
@@ -1179,7 +1179,7 @@
       <c r="U13" s="3"/>
     </row>
     <row r="14" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="9">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1187,7 +1187,9 @@
       <c r="C14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="5"/>
+      <c r="D14" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -1207,15 +1209,15 @@
       <c r="U14" s="3"/>
     </row>
     <row r="15" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="6">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="26" t="s">
         <v>77</v>
       </c>
       <c r="E15" s="8"/>
@@ -1237,7 +1239,7 @@
       <c r="U15" s="3"/>
     </row>
     <row r="16" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="9">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1245,7 +1247,7 @@
       <c r="C16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="25" t="s">
         <v>77</v>
       </c>
       <c r="E16" s="5"/>
@@ -1267,7 +1269,7 @@
       <c r="U16" s="3"/>
     </row>
     <row r="17" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1275,7 +1277,9 @@
       <c r="C17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
@@ -1295,7 +1299,7 @@
       <c r="U17" s="3"/>
     </row>
     <row r="18" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="9">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1303,7 +1307,7 @@
       <c r="C18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="25" t="s">
         <v>77</v>
       </c>
       <c r="E18" s="5"/>
@@ -1325,7 +1329,7 @@
       <c r="U18" s="3"/>
     </row>
     <row r="19" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1333,7 +1337,7 @@
       <c r="C19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="26" t="s">
         <v>77</v>
       </c>
       <c r="E19" s="8"/>
@@ -1355,7 +1359,7 @@
       <c r="U19" s="3"/>
     </row>
     <row r="20" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="9">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1363,7 +1367,7 @@
       <c r="C20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="25" t="s">
         <v>77</v>
       </c>
       <c r="E20" s="5"/>
@@ -1385,7 +1389,7 @@
       <c r="U20" s="3"/>
     </row>
     <row r="21" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1393,7 +1397,7 @@
       <c r="C21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="26" t="s">
         <v>77</v>
       </c>
       <c r="E21" s="8"/>
@@ -1415,7 +1419,7 @@
       <c r="U21" s="3"/>
     </row>
     <row r="22" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="9">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1423,7 +1427,7 @@
       <c r="C22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="25" t="s">
         <v>77</v>
       </c>
       <c r="E22" s="5"/>
@@ -1445,7 +1449,7 @@
       <c r="U22" s="3"/>
     </row>
     <row r="23" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1453,7 +1457,7 @@
       <c r="C23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="36" t="s">
+      <c r="D23" s="26" t="s">
         <v>77</v>
       </c>
       <c r="E23" s="8"/>
@@ -1475,7 +1479,7 @@
       <c r="U23" s="3"/>
     </row>
     <row r="24" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="35" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="9">
@@ -1485,7 +1489,9 @@
       <c r="C24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="5"/>
+      <c r="D24" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -1505,7 +1511,7 @@
       <c r="U24" s="3"/>
     </row>
     <row r="25" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1513,7 +1519,9 @@
       <c r="C25" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
@@ -1533,15 +1541,17 @@
       <c r="U25" s="3"/>
     </row>
     <row r="26" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="9">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="5"/>
+      <c r="D26" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -1561,7 +1571,7 @@
       <c r="U26" s="3"/>
     </row>
     <row r="27" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1569,7 +1579,9 @@
       <c r="C27" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="8"/>
+      <c r="D27" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -1589,7 +1601,7 @@
       <c r="U27" s="3"/>
     </row>
     <row r="28" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="27" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="9">
@@ -1599,7 +1611,9 @@
       <c r="C28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="5"/>
+      <c r="D28" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -1619,7 +1633,7 @@
       <c r="U28" s="3"/>
     </row>
     <row r="29" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="6">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1627,7 +1641,9 @@
       <c r="C29" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="8"/>
+      <c r="D29" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
@@ -1647,7 +1663,7 @@
       <c r="U29" s="3"/>
     </row>
     <row r="30" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="9">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1655,7 +1671,7 @@
       <c r="C30" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="25" t="s">
         <v>77</v>
       </c>
       <c r="E30" s="5"/>
@@ -1677,7 +1693,7 @@
       <c r="U30" s="3"/>
     </row>
     <row r="31" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="35" t="s">
         <v>40</v>
       </c>
       <c r="B31" s="6">
@@ -1687,7 +1703,9 @@
       <c r="C31" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="8"/>
+      <c r="D31" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
@@ -1707,7 +1725,7 @@
       <c r="U31" s="3"/>
     </row>
     <row r="32" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="9">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1715,7 +1733,9 @@
       <c r="C32" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="5"/>
+      <c r="D32" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -1735,7 +1755,7 @@
       <c r="U32" s="3"/>
     </row>
     <row r="33" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="6">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1743,7 +1763,9 @@
       <c r="C33" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="8"/>
+      <c r="D33" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
@@ -1763,7 +1785,7 @@
       <c r="U33" s="3"/>
     </row>
     <row r="34" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="9">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1771,7 +1793,9 @@
       <c r="C34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="5"/>
+      <c r="D34" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -1791,7 +1815,7 @@
       <c r="U34" s="3"/>
     </row>
     <row r="35" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="6">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1799,7 +1823,9 @@
       <c r="C35" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="8"/>
+      <c r="D35" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
@@ -1819,7 +1845,7 @@
       <c r="U35" s="3"/>
     </row>
     <row r="36" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
+      <c r="A36" s="28"/>
       <c r="B36" s="9">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1827,7 +1853,9 @@
       <c r="C36" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="5"/>
+      <c r="D36" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -1847,7 +1875,7 @@
       <c r="U36" s="3"/>
     </row>
     <row r="37" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="6">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1855,7 +1883,9 @@
       <c r="C37" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="8"/>
+      <c r="D37" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
@@ -1875,7 +1905,7 @@
       <c r="U37" s="3"/>
     </row>
     <row r="38" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B38" s="9">
@@ -1885,7 +1915,9 @@
       <c r="C38" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="5"/>
+      <c r="D38" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
@@ -1905,7 +1937,7 @@
       <c r="U38" s="3"/>
     </row>
     <row r="39" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="6">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1913,7 +1945,9 @@
       <c r="C39" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="8"/>
+      <c r="D39" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
@@ -1933,7 +1967,7 @@
       <c r="U39" s="3"/>
     </row>
     <row r="40" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
+      <c r="A40" s="28"/>
       <c r="B40" s="9">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1941,7 +1975,9 @@
       <c r="C40" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="5"/>
+      <c r="D40" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -1961,7 +1997,7 @@
       <c r="U40" s="3"/>
     </row>
     <row r="41" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="6">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1969,7 +2005,9 @@
       <c r="C41" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="8"/>
+      <c r="D41" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
@@ -1989,7 +2027,7 @@
       <c r="U41" s="3"/>
     </row>
     <row r="42" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="9">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1997,7 +2035,9 @@
       <c r="C42" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="5"/>
+      <c r="D42" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
@@ -2017,7 +2057,7 @@
       <c r="U42" s="3"/>
     </row>
     <row r="43" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="6">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2025,7 +2065,9 @@
       <c r="C43" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D43" s="8"/>
+      <c r="D43" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
@@ -2045,7 +2087,7 @@
       <c r="U43" s="3"/>
     </row>
     <row r="44" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
+      <c r="A44" s="28"/>
       <c r="B44" s="9">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2053,7 +2095,9 @@
       <c r="C44" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D44" s="5"/>
+      <c r="D44" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
@@ -2073,7 +2117,7 @@
       <c r="U44" s="3"/>
     </row>
     <row r="45" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="29" t="s">
         <v>56</v>
       </c>
       <c r="B45" s="6">
@@ -2083,7 +2127,9 @@
       <c r="C45" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="8"/>
+      <c r="D45" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -2103,7 +2149,7 @@
       <c r="U45" s="3"/>
     </row>
     <row r="46" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
+      <c r="A46" s="28"/>
       <c r="B46" s="9">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2111,7 +2157,9 @@
       <c r="C46" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D46" s="5"/>
+      <c r="D46" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -2131,7 +2179,7 @@
       <c r="U46" s="3"/>
     </row>
     <row r="47" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
+      <c r="A47" s="28"/>
       <c r="B47" s="6">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2139,7 +2187,9 @@
       <c r="C47" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D47" s="8"/>
+      <c r="D47" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
@@ -2159,7 +2209,7 @@
       <c r="U47" s="3"/>
     </row>
     <row r="48" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
+      <c r="A48" s="28"/>
       <c r="B48" s="9">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2167,7 +2217,9 @@
       <c r="C48" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D48" s="5"/>
+      <c r="D48" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -2187,7 +2239,7 @@
       <c r="U48" s="3"/>
     </row>
     <row r="49" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
+      <c r="A49" s="28"/>
       <c r="B49" s="6">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2195,7 +2247,9 @@
       <c r="C49" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D49" s="8"/>
+      <c r="D49" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
@@ -2215,7 +2269,7 @@
       <c r="U49" s="3"/>
     </row>
     <row r="50" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B50" s="9">
@@ -2225,7 +2279,9 @@
       <c r="C50" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="5"/>
+      <c r="D50" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
@@ -2245,7 +2301,7 @@
       <c r="U50" s="3"/>
     </row>
     <row r="51" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
+      <c r="A51" s="28"/>
       <c r="B51" s="6">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2253,7 +2309,9 @@
       <c r="C51" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D51" s="8"/>
+      <c r="D51" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
@@ -2273,19 +2331,19 @@
       <c r="U51" s="3"/>
     </row>
     <row r="52" spans="1:21" ht="13" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B52" s="26"/>
+      <c r="B52" s="32"/>
       <c r="C52" s="11" t="s">
         <v>65</v>
       </c>
       <c r="D52" s="12">
-        <f t="shared" ref="D52:G52" si="1">COUNTIF(D2:D51,"OK")*100/50</f>
-        <v>42</v>
+        <f>COUNTIF(D2:D51,"OK")*80/50</f>
+        <v>80</v>
       </c>
       <c r="E52" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D52:G52" si="1">COUNTIF(E2:E51,"OK")*100/50</f>
         <v>0</v>
       </c>
       <c r="F52" s="13">
@@ -2349,23 +2407,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -2598,23 +2656,23 @@
       <c r="W9" s="3"/>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>

</xml_diff>